<commit_message>
Now conducts a test on whether the company has had positive earnings in the past 10 years
</commit_message>
<xml_diff>
--- a/written_files/errors_with_debug_notes.xlsx
+++ b/written_files/errors_with_debug_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlson\PycharmProjects\grahamBot\written_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A556149-F2DD-4408-A8AB-02EA990825FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{FD3FE98E-39EC-4E90-A30C-4DDC71E9C82F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28020" yWindow="1695" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="errors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="56">
   <si>
     <t>rank</t>
   </si>
@@ -134,6 +134,60 @@
   </si>
   <si>
     <t>Polaris Industries</t>
+  </si>
+  <si>
+    <t>My notes</t>
+  </si>
+  <si>
+    <t>Could not be found with both words, but could be found with just 'Polaris' on marketwatch as Polaris Inc.</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>They changed their name to Polaris Inc. in July 2019</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>They were purchased by Cleveland Cliffs</t>
+  </si>
+  <si>
+    <t>Could be found using 'Packaging Corp.' and 'Packaging' on marketwatch</t>
+  </si>
+  <si>
+    <t>Not publicly traded</t>
+  </si>
+  <si>
+    <t>Just 'newmont' works on marketwatch</t>
+  </si>
+  <si>
+    <t>They are a mutual insurance company, so not publicly traded</t>
+  </si>
+  <si>
+    <t>Can be found through 'erie' on marketwatch then scanning page for ' erie ' word</t>
+  </si>
+  <si>
+    <t>Erie Insurance Group is the parent of erie indemnity company</t>
+  </si>
+  <si>
+    <t>O'Reilly Automotive</t>
+  </si>
+  <si>
+    <t>could not find info on macrotrends</t>
+  </si>
+  <si>
+    <t>Can't use macrotrends, need backup website, only work on backup if there are lots of this error</t>
+  </si>
+  <si>
+    <t>Use backup algorithm on market watch or use backup website</t>
+  </si>
+  <si>
+    <t>they were acquired by wesco international 'WCC'</t>
+  </si>
+  <si>
+    <t>Not publicly traded, also called (edward jones)</t>
   </si>
 </sst>
 </file>
@@ -974,13 +1028,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="96" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -990,8 +1054,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>36</v>
       </c>
@@ -1002,7 +1075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>46</v>
       </c>
@@ -1013,7 +1086,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>71</v>
       </c>
@@ -1024,7 +1097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>73</v>
       </c>
@@ -1035,7 +1108,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>75</v>
       </c>
@@ -1046,7 +1119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>84</v>
       </c>
@@ -1057,7 +1130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>91</v>
       </c>
@@ -1068,7 +1141,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>104</v>
       </c>
@@ -1079,7 +1152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>111</v>
       </c>
@@ -1090,7 +1163,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>201</v>
       </c>
@@ -1101,7 +1174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>212</v>
       </c>
@@ -1112,7 +1185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>237</v>
       </c>
@@ -1123,7 +1196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>244</v>
       </c>
@@ -1134,7 +1207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>270</v>
       </c>
@@ -1145,7 +1218,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>278</v>
       </c>
@@ -1156,7 +1229,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>285</v>
       </c>
@@ -1167,7 +1240,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>298</v>
       </c>
@@ -1178,7 +1251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>304</v>
       </c>
@@ -1189,7 +1262,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>306</v>
       </c>
@@ -1200,7 +1273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>332</v>
       </c>
@@ -1211,7 +1284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>336</v>
       </c>
@@ -1222,7 +1295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>340</v>
       </c>
@@ -1233,7 +1306,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>350</v>
       </c>
@@ -1244,7 +1317,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>351</v>
       </c>
@@ -1254,8 +1327,11 @@
       <c r="C25" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>356</v>
       </c>
@@ -1265,8 +1341,11 @@
       <c r="C26" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>364</v>
       </c>
@@ -1276,8 +1355,11 @@
       <c r="C27" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>381</v>
       </c>
@@ -1287,8 +1369,17 @@
       <c r="C28" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>382</v>
       </c>
@@ -1298,8 +1389,11 @@
       <c r="C29" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>419</v>
       </c>
@@ -1309,8 +1403,11 @@
       <c r="C30" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>423</v>
       </c>
@@ -1320,8 +1417,11 @@
       <c r="C31" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>432</v>
       </c>
@@ -1331,8 +1431,11 @@
       <c r="C32" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>443</v>
       </c>
@@ -1342,8 +1445,14 @@
       <c r="C33" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>476</v>
       </c>
@@ -1352,6 +1461,26 @@
       </c>
       <c r="C34" t="s">
         <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>329</v>
+      </c>
+      <c r="B35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>